<commit_message>
added weekly volume breakdown
</commit_message>
<xml_diff>
--- a/CAI_Workout_Regimen.xlsx
+++ b/CAI_Workout_Regimen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Everything_Else\CAI_Workout_Regimen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Desktop\CAI_Workout_Regimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232447BB-16B9-4DF0-AAF8-4B5268FE60B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A4640A-52BC-435C-A27C-13E2CBCC053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13068" yWindow="-2700" windowWidth="13176" windowHeight="22656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13068" yWindow="-2700" windowWidth="13176" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workout Plan" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="111">
   <si>
     <t>Day</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Back</t>
   </si>
   <si>
-    <t>Vertical Pull</t>
-  </si>
-  <si>
     <t>Pull-Up</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Lat Prayers</t>
   </si>
   <si>
-    <t>Horizontal Pull</t>
-  </si>
-  <si>
     <t>Seated Cable Row</t>
   </si>
   <si>
@@ -74,12 +68,6 @@
     <t>Cable Upright Row</t>
   </si>
   <si>
-    <t>Shoulders</t>
-  </si>
-  <si>
-    <t>Front Delt</t>
-  </si>
-  <si>
     <t>Machine Shoulder Press</t>
   </si>
   <si>
@@ -92,39 +80,21 @@
     <t>Isolation</t>
   </si>
   <si>
-    <t>Rear Delt</t>
-  </si>
-  <si>
     <t>Muscle Group</t>
   </si>
   <si>
-    <t>Sub-Group</t>
-  </si>
-  <si>
-    <t>Weekly Sets</t>
-  </si>
-  <si>
     <t>Chest</t>
   </si>
   <si>
-    <t>Arms</t>
-  </si>
-  <si>
     <t>Biceps</t>
   </si>
   <si>
     <t>Triceps</t>
   </si>
   <si>
-    <t>Legs</t>
-  </si>
-  <si>
     <t>Quads</t>
   </si>
   <si>
-    <t>Hamstrings/Glutes</t>
-  </si>
-  <si>
     <t>Calves</t>
   </si>
   <si>
@@ -273,6 +243,117 @@
   </si>
   <si>
     <t>Seated Calf Raise</t>
+  </si>
+  <si>
+    <t>Glutes</t>
+  </si>
+  <si>
+    <t>Front Delts</t>
+  </si>
+  <si>
+    <t>Side Delts</t>
+  </si>
+  <si>
+    <t>Rear Delts</t>
+  </si>
+  <si>
+    <t>Sets/Week</t>
+  </si>
+  <si>
+    <t>Exercise (Day &amp; Sets)</t>
+  </si>
+  <si>
+    <t>Traps</t>
+  </si>
+  <si>
+    <t>Total Sets/Week</t>
+  </si>
+  <si>
+    <t>Incline DB Bench Press – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Incline Bench Press – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Dips – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Incline DB Bench Press – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Machine Fly – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Back (Lats / Mid-Upper)</t>
+  </si>
+  <si>
+    <t>Pull-Up – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Seated Cable Row – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Chest Supported Row – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Lat Pulldown – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Lat Prayers – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Leg Extension – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Leg Press – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Smith Machine Squat – Day 2 (4)</t>
+  </si>
+  <si>
+    <t>Romanian Deadlift – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Barbell Back Extension – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Leg Curl – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Smith Machine Calf Raise – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Seated Calf Raise – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Machine Shoulder Press – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Cable Lateral Raise – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>Cable Upright Row – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Cable Lateral Raise – Day 4 (3)</t>
+  </si>
+  <si>
+    <t>Rear Delt Cable Fly – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Tricep Pushdown – Day 1 (3)</t>
+  </si>
+  <si>
+    <t>EZ-Bar Curl – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Dumbbell Bicep Curl – Day 3 (3)</t>
+  </si>
+  <si>
+    <t>Cable Crunch – Day 2 (3)</t>
+  </si>
+  <si>
+    <t>Leg Raises – Day 4 (3)</t>
   </si>
 </sst>
 </file>
@@ -617,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -646,10 +727,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -669,13 +750,13 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -686,19 +767,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -709,19 +790,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -732,19 +813,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -755,19 +836,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -778,19 +859,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -801,19 +882,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
         <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -824,19 +905,19 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -847,19 +928,19 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -876,13 +957,13 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -893,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -902,10 +983,10 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -916,19 +997,19 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -939,19 +1020,19 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -962,19 +1043,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -991,13 +1072,13 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1008,19 +1089,19 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1031,19 +1112,19 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1054,19 +1135,19 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1077,19 +1158,19 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1100,19 +1181,19 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1123,19 +1204,19 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
         <v>44</v>
-      </c>
-      <c r="F24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1152,13 +1233,13 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1169,19 +1250,19 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1198,13 +1279,13 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1215,19 +1296,19 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F29" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1238,19 +1319,19 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1261,19 +1342,19 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1284,19 +1365,19 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1306,148 +1387,462 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="C2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46">
         <v>18</v>
       </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11">
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G63">
         <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>80</v>
+      </c>
+      <c r="F66" t="s">
+        <v>103</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reordering exercises within each day. no changes made to types of exercises in the regimen.
</commit_message>
<xml_diff>
--- a/CAI_Workout_Regimen.xlsx
+++ b/CAI_Workout_Regimen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Desktop\CAI_Workout_Regimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A4640A-52BC-435C-A27C-13E2CBCC053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CDB93B-FFF7-4FBD-9B8E-4A00EC94C471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13068" yWindow="-2700" windowWidth="13176" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workout Plan" sheetId="3" r:id="rId1"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -753,10 +753,10 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -776,10 +776,10 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -790,19 +790,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -813,19 +813,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -951,19 +951,19 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -974,19 +974,19 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1020,19 +1020,19 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1043,19 +1043,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1066,19 +1066,19 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1089,19 +1089,19 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1135,16 +1135,16 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="G21" t="s">
         <v>39</v>
@@ -1158,16 +1158,16 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
         <v>39</v>
@@ -1227,19 +1227,19 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1250,19 +1250,19 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1282,10 +1282,10 @@
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1342,7 +1342,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1351,10 +1351,10 @@
         <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed order of exercises within each of the days
</commit_message>
<xml_diff>
--- a/CAI_Workout_Regimen.xlsx
+++ b/CAI_Workout_Regimen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Desktop\CAI_Workout_Regimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CDB93B-FFF7-4FBD-9B8E-4A00EC94C471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5827F27F-EF63-4C2B-8FB1-4F1326308C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -696,687 +696,688 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="B2:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G13" t="s">
         <v>58</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="C14">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G14" t="s">
         <v>48</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="B14">
+      <c r="C15">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
         <v>38</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G15" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="C16">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="B16">
+      <c r="C17">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
         <v>34</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G17" t="s">
         <v>21</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
         <v>34</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G19" t="s">
         <v>35</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
         <v>43</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G23" t="s">
         <v>56</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
         <v>31</v>
       </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="G28" t="s">
         <v>48</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>4</v>
-      </c>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>67</v>
       </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
         <v>38</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G30" t="s">
         <v>68</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
         <v>4</v>
       </c>
-      <c r="B30">
+      <c r="C31">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
         <v>73</v>
       </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
         <v>38</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G31" t="s">
         <v>24</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32">
         <v>4</v>
       </c>
-      <c r="B31">
+      <c r="C32">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
         <v>7</v>
       </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
         <v>38</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G32" t="s">
         <v>20</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33">
         <v>4</v>
       </c>
-      <c r="B32">
+      <c r="C33">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>69</v>
       </c>
-      <c r="D32">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
         <v>38</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G33" t="s">
         <v>70</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H33" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>